<commit_message>
feat: monthly based tables
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -1,33 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.lifantev/prsnl/bot/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEC8396-CCDC-DA41-AE48-7DF46363700F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +51,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -407,136 +353,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BD80DE-1FE1-1843-A0A3-C8AF36825483}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="11.33203125" customWidth="1" min="1" max="1"/>
-    <col width="20.33203125" customWidth="1" min="2" max="2"/>
-    <col width="19.5" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Timestamp</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>mgm_ru</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-02-07 23:16:22</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>mgm_ru</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-02-07 23:26:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>mgm_ru</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-02-07 23:28:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>mgm_ru</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2025-02-07 23:46:25</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>mgm_ru</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Check-in</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-02-07 23:53:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>mgm_ru</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Check-out</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-02-07 23:53:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>mgm_ru</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Check-in</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2025-02-08 00:00:56</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: vertically growing table done
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -1,38 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.lifantev/prsnl/bot/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEC8396-CCDC-DA41-AE48-7DF46363700F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="02-2025" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,23 +46,99 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="AttendanceTable" displayName="AttendanceTable" ref="A1:E2" headerRowCount="1">
+  <autoFilter ref="A1:E2"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Дата"/>
+    <tableColumn id="2" name="Username"/>
+    <tableColumn id="3" name="Время Check-in"/>
+    <tableColumn id="4" name="Время Check-out"/>
+    <tableColumn id="5" name="Рабочее время"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -353,12 +425,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BD80DE-1FE1-1843-A0A3-C8AF36825483}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Дата</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Время Check-in</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Время Check-out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Рабочее время</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>08-02-2025</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>fantdali</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>23:47</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>23:48</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>00:01</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: horizontally growing table
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -6,8 +6,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="02-2025" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2025-02" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -125,20 +125,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="AttendanceTable" displayName="AttendanceTable" ref="A1:E2" headerRowCount="1">
-  <autoFilter ref="A1:E2"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Дата"/>
-    <tableColumn id="2" name="Username"/>
-    <tableColumn id="3" name="Время Check-in"/>
-    <tableColumn id="4" name="Время Check-out"/>
-    <tableColumn id="5" name="Рабочее время"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,81 +416,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Дата</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Время Check-in</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Время Check-out</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Рабочее время</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>08-02-2025</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>fantdali</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>23:47</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>23:48</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>00:01</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </tableParts>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -514,14 +434,223 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="7" customWidth="1" min="2" max="2"/>
+    <col width="7" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="7" customWidth="1" min="5" max="5"/>
+    <col width="7" customWidth="1" min="6" max="6"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="8" max="8"/>
+    <col width="7" customWidth="1" min="9" max="9"/>
+    <col width="26" customWidth="1" min="10" max="10"/>
+    <col width="7" customWidth="1" min="11" max="11"/>
+    <col width="7" customWidth="1" min="12" max="12"/>
+    <col width="7" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="14" max="14"/>
+    <col width="7" customWidth="1" min="15" max="15"/>
+    <col width="7" customWidth="1" min="16" max="16"/>
+    <col width="7" customWidth="1" min="17" max="17"/>
+    <col width="7" customWidth="1" min="18" max="18"/>
+    <col width="7" customWidth="1" min="19" max="19"/>
+    <col width="7" customWidth="1" min="20" max="20"/>
+    <col width="7" customWidth="1" min="21" max="21"/>
+    <col width="7" customWidth="1" min="22" max="22"/>
+    <col width="7" customWidth="1" min="23" max="23"/>
+    <col width="7" customWidth="1" min="24" max="24"/>
+    <col width="7" customWidth="1" min="25" max="25"/>
+    <col width="7" customWidth="1" min="26" max="26"/>
+    <col width="7" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="28" max="28"/>
+    <col width="7" customWidth="1" min="29" max="29"/>
+    <col width="7" customWidth="1" min="30" max="30"/>
+    <col width="7" customWidth="1" min="31" max="31"/>
+    <col width="7" customWidth="1" min="32" max="32"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>fantdali</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>00:06 - 00:08 (00:02)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: google sheets core logic
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.lifantev/prsnl/bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2287C4A5-29A8-D949-861E-195E168B559D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55453B00-07A8-B645-8229-A14C3B5FAFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1104,16 +1104,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="CA1:CC1"/>
-    <mergeCell ref="AZ1:BB1"/>
-    <mergeCell ref="BL1:BN1"/>
-    <mergeCell ref="BR1:BT1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="AB1:AD1"/>
     <mergeCell ref="CG1:CI1"/>
     <mergeCell ref="AQ1:AS1"/>
     <mergeCell ref="AW1:AY1"/>
@@ -1130,6 +1120,16 @@
     <mergeCell ref="AN1:AP1"/>
     <mergeCell ref="Y1:AA1"/>
     <mergeCell ref="BU1:BW1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="CA1:CC1"/>
+    <mergeCell ref="AZ1:BB1"/>
+    <mergeCell ref="BL1:BN1"/>
+    <mergeCell ref="BR1:BT1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="AB1:AD1"/>
     <mergeCell ref="AE1:AG1"/>
     <mergeCell ref="AK1:AM1"/>
   </mergeCells>

</xml_diff>